<commit_message>
Fixed problems with calculating r from DDE time-series data
</commit_message>
<xml_diff>
--- a/Model results DI Tave.xlsx
+++ b/Model results DI Tave.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD28084-0396-9B40-959B-77B966BE1C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20F34AF-4CF5-6148-9E55-085C8074C05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6200" yWindow="500" windowWidth="22560" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model results" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -339,14 +339,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,14 +520,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -689,11 +677,22 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -742,30 +741,23 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1125,7 +1117,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+      <selection pane="topRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,70 +1125,72 @@
     <col min="1" max="1" width="44.83203125" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B2">
@@ -1211,52 +1205,52 @@
       <c r="E2">
         <v>0.13400000000000001</v>
       </c>
-      <c r="F2">
-        <v>0.127</v>
-      </c>
-      <c r="G2">
-        <v>0.108</v>
-      </c>
-      <c r="H2" s="8">
-        <v>0.127</v>
-      </c>
-      <c r="I2" s="6">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0.12</v>
-      </c>
-      <c r="K2" s="5">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="L2" s="9">
+      <c r="F2" s="1">
+        <v>0.12663366000000001</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.10765085000000001</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0.12731837882595601</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8.2553518417710497E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.12038421792211899</v>
+      </c>
+      <c r="K2" s="1">
+        <v>7.6048914264231299E-2</v>
+      </c>
+      <c r="L2" s="10">
         <f>H2/$E2</f>
-        <v>0.94776119402985071</v>
-      </c>
-      <c r="M2" s="14">
+        <v>0.95013715541758215</v>
+      </c>
+      <c r="M2" s="15">
         <f>I2/$E2</f>
-        <v>0.61940298507462688</v>
-      </c>
-      <c r="N2" s="14">
+        <v>0.61607103296798871</v>
+      </c>
+      <c r="N2" s="15">
         <f>J2/$F2</f>
-        <v>0.94488188976377951</v>
-      </c>
-      <c r="O2" s="16">
+        <v>0.95064943966808657</v>
+      </c>
+      <c r="O2" s="15">
         <f>K2/$F2</f>
-        <v>0.59842519685039364</v>
-      </c>
-      <c r="P2" s="1">
+        <v>0.6005426540165647</v>
+      </c>
+      <c r="P2" s="10">
         <f>M2-L2</f>
-        <v>-0.32835820895522383</v>
+        <v>-0.33406612244959344</v>
       </c>
       <c r="Q2" s="1">
         <f>O2-N2</f>
-        <v>-0.34645669291338588</v>
-      </c>
-      <c r="R2" s="7"/>
+        <v>-0.35010678565152187</v>
+      </c>
+      <c r="R2" s="5"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B3">
@@ -1271,52 +1265,52 @@
       <c r="E3">
         <v>0.154</v>
       </c>
-      <c r="F3">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="G3">
-        <v>0.157</v>
-      </c>
-      <c r="H3" s="9">
-        <v>0.125</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0.152</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="L3" s="9">
+      <c r="F3" s="1">
+        <v>0.13206163000000001</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.15710431</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.12525969272089099</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.152411101117542</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.115964603746277</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.14839017736941401</v>
+      </c>
+      <c r="L3" s="6">
         <f t="shared" ref="L3:L28" si="0">H3/$E3</f>
-        <v>0.81168831168831168</v>
+        <v>0.81337462805773375</v>
       </c>
       <c r="M3" s="14">
         <f t="shared" ref="M3:M28" si="1">I3/$E3</f>
-        <v>0.98701298701298701</v>
+        <v>0.98968247478923377</v>
       </c>
       <c r="N3" s="14">
         <f t="shared" ref="N3:N28" si="2">J3/$F3</f>
-        <v>0.87878787878787878</v>
-      </c>
-      <c r="O3" s="16">
+        <v>0.87810974123427821</v>
+      </c>
+      <c r="O3" s="14">
         <f t="shared" ref="O3:O28" si="3">K3/$F3</f>
-        <v>1.1212121212121211</v>
-      </c>
-      <c r="P3" s="1">
+        <v>1.1236433880864107</v>
+      </c>
+      <c r="P3" s="6">
         <f t="shared" ref="P3:P28" si="4">M3-L3</f>
-        <v>0.17532467532467533</v>
+        <v>0.17630784673150002</v>
       </c>
       <c r="Q3" s="1">
         <f t="shared" ref="Q3:Q28" si="5">O3-N3</f>
-        <v>0.24242424242424232</v>
-      </c>
-      <c r="R3" s="7"/>
+        <v>0.24553364685213253</v>
+      </c>
+      <c r="R3" s="5"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B4">
@@ -1331,52 +1325,52 @@
       <c r="E4">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="F4">
-        <v>0.182</v>
-      </c>
-      <c r="G4">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="H4" s="9">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="I4" s="6">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.159</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0.193</v>
-      </c>
-      <c r="L4" s="9">
+      <c r="F4" s="1">
+        <v>0.18165244</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.20334092000000001</v>
+      </c>
+      <c r="H4" s="6">
+        <v>7.8510611435261501E-2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>8.6862101687714993E-2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.15893208982440499</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.19348343021677</v>
+      </c>
+      <c r="L4" s="6">
         <f t="shared" si="0"/>
-        <v>0.89772727272727282</v>
+        <v>0.8921660390370626</v>
       </c>
       <c r="M4" s="14">
         <f t="shared" si="1"/>
-        <v>0.98863636363636365</v>
+        <v>0.9870693373603977</v>
       </c>
       <c r="N4" s="14">
         <f t="shared" si="2"/>
-        <v>0.87362637362637363</v>
-      </c>
-      <c r="O4" s="16">
+        <v>0.87492405730638678</v>
+      </c>
+      <c r="O4" s="14">
         <f t="shared" si="3"/>
-        <v>1.0604395604395604</v>
-      </c>
-      <c r="P4" s="1">
+        <v>1.0651298172310264</v>
+      </c>
+      <c r="P4" s="6">
         <f t="shared" si="4"/>
-        <v>9.0909090909090828E-2</v>
+        <v>9.4903298323335106E-2</v>
       </c>
       <c r="Q4" s="1">
         <f t="shared" si="5"/>
-        <v>0.18681318681318682</v>
-      </c>
-      <c r="R4" s="7"/>
+        <v>0.19020575992463962</v>
+      </c>
+      <c r="R4" s="5"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B5">
@@ -1391,52 +1385,52 @@
       <c r="E5">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="F5">
-        <v>0.104</v>
-      </c>
-      <c r="G5">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="H5" s="8">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="I5" s="6">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="J5" s="6">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="K5" s="6">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="L5" s="9">
+      <c r="F5" s="1">
+        <v>0.10366649</v>
+      </c>
+      <c r="G5" s="1">
+        <v>9.1435240000000001E-2</v>
+      </c>
+      <c r="H5" s="6">
+        <v>8.1424481388495507E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>8.2125942356189599E-2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>9.0818270162646597E-2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>4.9424462239443898E-2</v>
+      </c>
+      <c r="L5" s="6">
         <f t="shared" si="0"/>
-        <v>0.92045454545454553</v>
+        <v>0.92527819759653995</v>
       </c>
       <c r="M5" s="14">
         <f t="shared" si="1"/>
-        <v>0.93181818181818188</v>
+        <v>0.93324934495670009</v>
       </c>
       <c r="N5" s="14">
         <f t="shared" si="2"/>
-        <v>0.875</v>
-      </c>
-      <c r="O5" s="16">
+        <v>0.87606197685140685</v>
+      </c>
+      <c r="O5" s="14">
         <f t="shared" si="3"/>
-        <v>0.4711538461538462</v>
-      </c>
-      <c r="P5" s="1">
+        <v>0.47676411383701617</v>
+      </c>
+      <c r="P5" s="6">
         <f t="shared" si="4"/>
-        <v>1.1363636363636354E-2</v>
+        <v>7.9711473601601357E-3</v>
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="5"/>
-        <v>-0.4038461538461538</v>
-      </c>
-      <c r="R5" s="7"/>
+        <v>-0.39929786301439069</v>
+      </c>
+      <c r="R5" s="5"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6">
@@ -1451,54 +1445,54 @@
       <c r="E6">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F6" s="21">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="G6">
-        <v>0.106</v>
-      </c>
-      <c r="H6" s="9">
-        <v>0.104</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0.109</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.122</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="L6" s="9">
-        <f>H6/$E6</f>
-        <v>0.63030303030303025</v>
+      <c r="F6" s="1">
+        <v>0.69928478000000005</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.10563027</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.10430294110273799</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.10871623810685201</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.122174904593252</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.100827073228625</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.63213903698629081</v>
       </c>
       <c r="M6" s="14">
-        <f>I6/$E6</f>
-        <v>0.66060606060606053</v>
+        <f t="shared" si="1"/>
+        <v>0.65888629155667877</v>
       </c>
       <c r="N6" s="14">
-        <f>J6/$F6</f>
-        <v>0.17453505007153078</v>
-      </c>
-      <c r="O6" s="16">
-        <f>K6/$F6</f>
-        <v>0.14449213161659516</v>
-      </c>
-      <c r="P6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.17471409086474327</v>
+      </c>
+      <c r="O6" s="14">
+        <f t="shared" si="3"/>
+        <v>0.14418599705348226</v>
+      </c>
+      <c r="P6" s="6">
         <f t="shared" si="4"/>
-        <v>3.0303030303030276E-2</v>
+        <v>2.6747254570387957E-2</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="5"/>
-        <v>-3.0042918454935619E-2</v>
-      </c>
-      <c r="R6" s="7" t="s">
+        <v>-3.0528093811261009E-2</v>
+      </c>
+      <c r="R6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -1513,54 +1507,54 @@
       <c r="E7">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F7" s="21">
-        <v>0.60299999999999998</v>
-      </c>
-      <c r="G7">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="H7" s="9">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="I7" s="6">
-        <v>6.3E-2</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="K7" s="6">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="L7" s="9">
+      <c r="F7" s="1">
+        <v>0.60309159999999995</v>
+      </c>
+      <c r="G7" s="1">
+        <v>9.6362030000000001E-2</v>
+      </c>
+      <c r="H7" s="6">
+        <v>5.2348278689079902E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>6.2759357974109004E-2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.119398993779794</v>
+      </c>
+      <c r="K7" s="1">
+        <v>8.4682789106848705E-2</v>
+      </c>
+      <c r="L7" s="6">
         <f t="shared" si="0"/>
-        <v>0.62650602409638545</v>
+        <v>0.6307021528804807</v>
       </c>
       <c r="M7" s="14">
         <f t="shared" si="1"/>
-        <v>0.75903614457831325</v>
+        <v>0.75613684306155426</v>
       </c>
       <c r="N7" s="14">
         <f t="shared" si="2"/>
-        <v>0.19734660033167495</v>
-      </c>
-      <c r="O7" s="16">
+        <v>0.19797820725706347</v>
+      </c>
+      <c r="O7" s="14">
         <f t="shared" si="3"/>
-        <v>0.14096185737976785</v>
-      </c>
-      <c r="P7" s="1">
+        <v>0.14041447287086856</v>
+      </c>
+      <c r="P7" s="6">
         <f t="shared" si="4"/>
-        <v>0.1325301204819278</v>
+        <v>0.12543469018107356</v>
       </c>
       <c r="Q7" s="1">
         <f t="shared" si="5"/>
-        <v>-5.6384742951907096E-2</v>
-      </c>
-      <c r="R7" s="7" t="s">
+        <v>-5.7563734386194915E-2</v>
+      </c>
+      <c r="R7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B8">
@@ -1575,54 +1569,54 @@
       <c r="E8">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F8" s="21">
-        <v>0.63800000000000001</v>
-      </c>
-      <c r="G8">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="H8" s="8">
-        <v>0.105</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0.187</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0.254</v>
-      </c>
-      <c r="L8" s="9">
+      <c r="F8" s="1">
+        <v>0.63848594000000003</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.74006145999999995</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.105298145941686</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.116262916209933</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.186926632159717</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.24501068445337701</v>
+      </c>
+      <c r="L8" s="6">
         <f t="shared" si="0"/>
-        <v>0.63636363636363635</v>
+        <v>0.63817058146476358</v>
       </c>
       <c r="M8" s="14">
         <f t="shared" si="1"/>
-        <v>0.70303030303030301</v>
+        <v>0.70462373460565453</v>
       </c>
       <c r="N8" s="14">
         <f t="shared" si="2"/>
-        <v>0.29310344827586204</v>
-      </c>
-      <c r="O8" s="16">
+        <v>0.29276546349590249</v>
+      </c>
+      <c r="O8" s="14">
         <f t="shared" si="3"/>
-        <v>0.39811912225705332</v>
-      </c>
-      <c r="P8" s="1">
+        <v>0.38373700829399154</v>
+      </c>
+      <c r="P8" s="6">
         <f t="shared" si="4"/>
-        <v>6.6666666666666652E-2</v>
+        <v>6.6453153140890953E-2</v>
       </c>
       <c r="Q8" s="1">
         <f t="shared" si="5"/>
-        <v>0.10501567398119127</v>
-      </c>
-      <c r="R8" s="7" t="s">
+        <v>9.0971544798089055E-2</v>
+      </c>
+      <c r="R8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B9">
@@ -1637,54 +1631,54 @@
       <c r="E9">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F9" s="21">
-        <v>0.67800000000000005</v>
+      <c r="F9" s="1">
+        <v>0.67801462000000001</v>
       </c>
       <c r="G9" s="1">
-        <v>0.28399999999999997</v>
-      </c>
-      <c r="H9" s="9">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="I9" s="6">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="K9" s="5">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="L9" s="9">
+        <v>0.75918889000000001</v>
+      </c>
+      <c r="H9" s="6">
+        <v>5.3773997470387198E-2</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5.44403628677795E-2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.13774874366495701</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.117923832857289</v>
+      </c>
+      <c r="L9" s="6">
         <f t="shared" si="0"/>
-        <v>0.6506024096385542</v>
+        <v>0.64787948759502645</v>
       </c>
       <c r="M9" s="14">
         <f t="shared" si="1"/>
-        <v>0.6506024096385542</v>
+        <v>0.65590798635878911</v>
       </c>
       <c r="N9" s="14">
         <f t="shared" si="2"/>
-        <v>0.20353982300884957</v>
-      </c>
-      <c r="O9" s="16">
+        <v>0.203164857514366</v>
+      </c>
+      <c r="O9" s="14">
         <f t="shared" si="3"/>
-        <v>0.17109144542772861</v>
-      </c>
-      <c r="P9" s="1">
+        <v>0.17392520659405397</v>
+      </c>
+      <c r="P9" s="6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8.0284987637626593E-3</v>
       </c>
       <c r="Q9" s="1">
         <f t="shared" si="5"/>
-        <v>-3.2448377581120957E-2</v>
-      </c>
-      <c r="R9" s="7" t="s">
+        <v>-2.9239650920312027E-2</v>
+      </c>
+      <c r="R9" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B10">
@@ -1700,51 +1694,51 @@
         <v>0.246</v>
       </c>
       <c r="F10" s="1">
-        <v>0.69</v>
-      </c>
-      <c r="G10">
-        <v>0.67600000000000005</v>
-      </c>
-      <c r="H10" s="9">
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0.215</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0.66</v>
-      </c>
-      <c r="K10" s="5">
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="L10" s="9">
+        <v>0.69314717999999997</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.68219817000000005</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.187555534029691</v>
+      </c>
+      <c r="I10" s="1">
+        <v>8.9563599045517403E-2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.65640953900830401</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.59114586140446401</v>
+      </c>
+      <c r="L10" s="6">
         <f t="shared" si="0"/>
-        <v>0.95121951219512202</v>
+        <v>0.76242087003939429</v>
       </c>
       <c r="M10" s="14">
         <f t="shared" si="1"/>
-        <v>0.87398373983739841</v>
+        <v>0.36407967091673743</v>
       </c>
       <c r="N10" s="14">
         <f t="shared" si="2"/>
-        <v>0.95652173913043492</v>
-      </c>
-      <c r="O10" s="16">
+        <v>0.94699878748450517</v>
+      </c>
+      <c r="O10" s="14">
         <f t="shared" si="3"/>
-        <v>0.67246376811594211</v>
-      </c>
-      <c r="P10" s="1">
+        <v>0.85284320337920738</v>
+      </c>
+      <c r="P10" s="6">
         <f t="shared" si="4"/>
-        <v>-7.7235772357723609E-2</v>
+        <v>-0.39834119912265686</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="5"/>
-        <v>-0.28405797101449282</v>
-      </c>
-      <c r="R10" s="7"/>
+        <v>-9.4155584105297785E-2</v>
+      </c>
+      <c r="R10" s="5"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B11">
@@ -1759,52 +1753,52 @@
       <c r="E11">
         <v>0.25700000000000001</v>
       </c>
-      <c r="F11">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="G11">
-        <v>0.69499999999999995</v>
-      </c>
-      <c r="H11" s="9">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0.19600000000000001</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0.379</v>
-      </c>
-      <c r="L11" s="9">
+      <c r="F11" s="1">
+        <v>0.72593700000000005</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.70309750999999998</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.146646382815764</v>
+      </c>
+      <c r="I11" s="1">
+        <v>-2.6436037366879099E-2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.68685766697440798</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.55110091358953095</v>
+      </c>
+      <c r="L11" s="6">
         <f t="shared" si="0"/>
-        <v>0.9377431906614786</v>
+        <v>0.57060849344655251</v>
       </c>
       <c r="M11" s="14">
         <f t="shared" si="1"/>
-        <v>0.76264591439688723</v>
+        <v>-0.10286395862598871</v>
       </c>
       <c r="N11" s="14">
         <f t="shared" si="2"/>
-        <v>0.94736842105263164</v>
-      </c>
-      <c r="O11" s="16">
+        <v>0.9461670461409295</v>
+      </c>
+      <c r="O11" s="14">
         <f t="shared" si="3"/>
-        <v>0.52493074792243766</v>
-      </c>
-      <c r="P11" s="1">
+        <v>0.75915804482969029</v>
+      </c>
+      <c r="P11" s="6">
         <f t="shared" si="4"/>
-        <v>-0.17509727626459137</v>
+        <v>-0.67347245207254125</v>
       </c>
       <c r="Q11" s="1">
         <f t="shared" si="5"/>
-        <v>-0.42243767313019398</v>
-      </c>
-      <c r="R11" s="7"/>
+        <v>-0.18700900131123921</v>
+      </c>
+      <c r="R11" s="5"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B12">
@@ -1819,52 +1813,52 @@
       <c r="E12">
         <v>0.249</v>
       </c>
-      <c r="F12">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="G12">
-        <v>0.77400000000000002</v>
-      </c>
-      <c r="H12" s="8">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0.73599999999999999</v>
-      </c>
-      <c r="K12" s="5">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="L12" s="9">
+      <c r="F12" s="1">
+        <v>0.78484485000000004</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.77745428999999999</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.23084497902259199</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.196565708507731</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.73036700867287496</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.55772034305604901</v>
+      </c>
+      <c r="L12" s="6">
         <f t="shared" si="0"/>
-        <v>0.92771084337349408</v>
+        <v>0.92708826916703613</v>
       </c>
       <c r="M12" s="14">
         <f t="shared" si="1"/>
-        <v>0.79116465863453822</v>
+        <v>0.78942051609530528</v>
       </c>
       <c r="N12" s="14">
         <f t="shared" si="2"/>
-        <v>0.94238156209987189</v>
-      </c>
-      <c r="O12" s="16">
+        <v>0.93058775715082409</v>
+      </c>
+      <c r="O12" s="14">
         <f t="shared" si="3"/>
-        <v>0.70038412291933416</v>
-      </c>
-      <c r="P12" s="1">
+        <v>0.71061222234693766</v>
+      </c>
+      <c r="P12" s="6">
         <f t="shared" si="4"/>
-        <v>-0.13654618473895586</v>
+        <v>-0.13766775307173085</v>
       </c>
       <c r="Q12" s="1">
         <f t="shared" si="5"/>
-        <v>-0.24199743918053773</v>
-      </c>
-      <c r="R12" s="7"/>
+        <v>-0.21997553480388643</v>
+      </c>
+      <c r="R12" s="5"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B13">
@@ -1880,53 +1874,53 @@
         <v>0.1</v>
       </c>
       <c r="F13" s="1">
-        <v>0.14000000000000001</v>
+        <v>0.40574658000000002</v>
       </c>
       <c r="G13" s="1">
-        <v>0.192</v>
-      </c>
-      <c r="H13" s="10">
-        <v>5.8999999999999997E-2</v>
+        <v>0.82672962999999999</v>
+      </c>
+      <c r="H13" s="6">
+        <v>6.9977115378766705E-2</v>
       </c>
       <c r="I13" s="1">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="J13" s="3">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="K13" s="4">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="L13" s="9">
+        <v>9.1284855154564803E-2</v>
+      </c>
+      <c r="J13" s="1">
+        <v>8.4228403473846594E-2</v>
+      </c>
+      <c r="K13" s="1">
+        <v>5.87483104190702E-2</v>
+      </c>
+      <c r="L13" s="6">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.69977115378766697</v>
       </c>
       <c r="M13" s="14">
         <f t="shared" si="1"/>
-        <v>0.34</v>
+        <v>0.91284855154564803</v>
       </c>
       <c r="N13" s="14">
         <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-      <c r="O13" s="16">
+        <v>0.20758869606207547</v>
+      </c>
+      <c r="O13" s="14">
         <f t="shared" si="3"/>
-        <v>0.5357142857142857</v>
-      </c>
-      <c r="P13" s="1">
+        <v>0.14479064843644571</v>
+      </c>
+      <c r="P13" s="6">
         <f t="shared" si="4"/>
-        <v>-0.24999999999999994</v>
+        <v>0.21307739775798107</v>
       </c>
       <c r="Q13" s="1">
         <f t="shared" si="5"/>
-        <v>-6.4285714285714279E-2</v>
-      </c>
-      <c r="R13" s="7" t="s">
+        <v>-6.2798047625629766E-2</v>
+      </c>
+      <c r="R13" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B14">
@@ -1941,54 +1935,54 @@
       <c r="E14">
         <v>0.104</v>
       </c>
-      <c r="F14">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="G14">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="H14" s="10">
-        <v>5.8999999999999997E-2</v>
+      <c r="F14" s="1">
+        <v>0.44737850000000001</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.62939641000000002</v>
+      </c>
+      <c r="H14" s="6">
+        <v>6.8920451059143198E-2</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="3">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="K14" s="4">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="L14" s="9">
+        <v>9.2856999983237307E-2</v>
+      </c>
+      <c r="J14" s="1">
+        <v>8.7584801372048299E-2</v>
+      </c>
+      <c r="K14" s="1">
+        <v>5.9767680044288299E-2</v>
+      </c>
+      <c r="L14" s="6">
         <f t="shared" si="0"/>
-        <v>0.56730769230769229</v>
+        <v>0.66269664479945389</v>
       </c>
       <c r="M14" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.89285576906958952</v>
       </c>
       <c r="N14" s="14">
         <f t="shared" si="2"/>
-        <v>0.58783783783783783</v>
-      </c>
-      <c r="O14" s="16">
+        <v>0.19577338064312053</v>
+      </c>
+      <c r="O14" s="14">
         <f t="shared" si="3"/>
-        <v>0.5067567567567568</v>
-      </c>
-      <c r="P14" s="1">
+        <v>0.13359533380412403</v>
+      </c>
+      <c r="P14" s="6">
         <f t="shared" si="4"/>
-        <v>-0.56730769230769229</v>
+        <v>0.23015912427013563</v>
       </c>
       <c r="Q14" s="1">
         <f t="shared" si="5"/>
-        <v>-8.108108108108103E-2</v>
-      </c>
-      <c r="R14" s="7" t="s">
+        <v>-6.2178046838996498E-2</v>
+      </c>
+      <c r="R14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B15">
@@ -2003,54 +1997,54 @@
       <c r="E15">
         <v>0.28599999999999998</v>
       </c>
-      <c r="F15">
-        <v>0.44900000000000001</v>
-      </c>
-      <c r="G15">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="H15" s="10">
-        <v>0.124</v>
+      <c r="F15" s="1">
+        <v>0.52944318000000001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.35986415999999999</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.123716186327014</v>
       </c>
       <c r="I15" s="1">
-        <v>0.154</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="L15" s="9">
+        <v>0.15419010882636799</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.27898550242516801</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.16311522763318101</v>
+      </c>
+      <c r="L15" s="6">
         <f t="shared" si="0"/>
-        <v>0.4335664335664336</v>
+        <v>0.43257407806648257</v>
       </c>
       <c r="M15" s="14">
         <f t="shared" si="1"/>
-        <v>0.53846153846153855</v>
+        <v>0.5391262546376504</v>
       </c>
       <c r="N15" s="14">
         <f t="shared" si="2"/>
-        <v>0.57238307349665929</v>
-      </c>
-      <c r="O15" s="16">
+        <v>0.52694134699245343</v>
+      </c>
+      <c r="O15" s="14">
         <f t="shared" si="3"/>
-        <v>0.36080178173719379</v>
-      </c>
-      <c r="P15" s="1">
+        <v>0.30808825912760085</v>
+      </c>
+      <c r="P15" s="6">
         <f t="shared" si="4"/>
-        <v>0.10489510489510495</v>
+        <v>0.10655217657116783</v>
       </c>
       <c r="Q15" s="3">
         <f t="shared" si="5"/>
-        <v>-0.2115812917594655</v>
-      </c>
-      <c r="R15" s="7" t="s">
+        <v>-0.21885308786485258</v>
+      </c>
+      <c r="R15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B16">
@@ -2065,54 +2059,54 @@
       <c r="E16">
         <v>0.19400000000000001</v>
       </c>
-      <c r="F16">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="G16">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="H16" s="10">
-        <v>0.161</v>
+      <c r="F16" s="1">
+        <v>0.13645921</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.11709559</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.16060537206138001</v>
       </c>
       <c r="I16" s="1">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0.109</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="L16" s="9">
+        <v>0.17517507209229799</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.108614356129535</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.10224855075163</v>
+      </c>
+      <c r="L16" s="6">
         <f t="shared" si="0"/>
-        <v>0.82989690721649489</v>
+        <v>0.82786274258443304</v>
       </c>
       <c r="M16" s="14">
         <f t="shared" si="1"/>
-        <v>0.902061855670103</v>
+        <v>0.9029642891355566</v>
       </c>
       <c r="N16" s="14">
         <f t="shared" si="2"/>
-        <v>0.80147058823529405</v>
-      </c>
-      <c r="O16" s="16">
+        <v>0.79594741996186991</v>
+      </c>
+      <c r="O16" s="14">
         <f t="shared" si="3"/>
-        <v>0.74999999999999989</v>
-      </c>
-      <c r="P16" s="1">
+        <v>0.74929754284544081</v>
+      </c>
+      <c r="P16" s="6">
         <f t="shared" si="4"/>
-        <v>7.2164948453608102E-2</v>
+        <v>7.5101546551123555E-2</v>
       </c>
       <c r="Q16" s="1">
         <f t="shared" si="5"/>
-        <v>-5.1470588235294157E-2</v>
-      </c>
-      <c r="R16" s="7" t="s">
+        <v>-4.6649877116429095E-2</v>
+      </c>
+      <c r="R16" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B17">
@@ -2127,54 +2121,54 @@
       <c r="E17">
         <v>0.443</v>
       </c>
-      <c r="F17">
-        <v>0.28299999999999997</v>
-      </c>
-      <c r="G17">
-        <v>0.249</v>
-      </c>
-      <c r="H17" s="10">
-        <v>0.40699999999999997</v>
+      <c r="F17" s="1">
+        <v>0.28768207000000001</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2.77753242</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.40741716795452299</v>
       </c>
       <c r="I17" s="1">
-        <v>0.378</v>
-      </c>
-      <c r="J17" s="3">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0.124</v>
-      </c>
-      <c r="L17" s="9">
+        <v>0.37804629555285701</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.263490062595441</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.12967835090687899</v>
+      </c>
+      <c r="L17" s="6">
         <f t="shared" si="0"/>
-        <v>0.91873589164785541</v>
+        <v>0.91967758003278322</v>
       </c>
       <c r="M17" s="14">
         <f t="shared" si="1"/>
-        <v>0.85327313769751689</v>
+        <v>0.8533776423315057</v>
       </c>
       <c r="N17" s="14">
         <f t="shared" si="2"/>
-        <v>0.93286219081272093</v>
-      </c>
-      <c r="O17" s="16">
+        <v>0.91590714219847269</v>
+      </c>
+      <c r="O17" s="14">
         <f t="shared" si="3"/>
-        <v>0.43816254416961137</v>
-      </c>
-      <c r="P17" s="1">
+        <v>0.4507696670386131</v>
+      </c>
+      <c r="P17" s="6">
         <f t="shared" si="4"/>
-        <v>-6.5462753950338515E-2</v>
+        <v>-6.6299937701277512E-2</v>
       </c>
       <c r="Q17" s="1">
         <f t="shared" si="5"/>
-        <v>-0.49469964664310956</v>
-      </c>
-      <c r="R17" s="7" t="s">
+        <v>-0.46513747515985959</v>
+      </c>
+      <c r="R17" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B18">
@@ -2189,54 +2183,54 @@
       <c r="E18">
         <v>0.30599999999999999</v>
       </c>
-      <c r="F18">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="G18">
-        <v>0.217</v>
-      </c>
-      <c r="H18" s="10">
-        <v>0.27</v>
+      <c r="F18" s="1">
+        <v>0.24686008000000001</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.22314355</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.269868765618971</v>
       </c>
       <c r="I18" s="1">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0.215</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="L18" s="9">
+        <v>0.271712902757478</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.214780090292569</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.198803283616558</v>
+      </c>
+      <c r="L18" s="6">
         <f t="shared" si="0"/>
-        <v>0.88235294117647067</v>
+        <v>0.88192407065023204</v>
       </c>
       <c r="M18" s="14">
         <f t="shared" si="1"/>
-        <v>0.88888888888888895</v>
+        <v>0.88795066260613731</v>
       </c>
       <c r="N18" s="14">
         <f t="shared" si="2"/>
-        <v>0.89211618257261416</v>
-      </c>
-      <c r="O18" s="16">
+        <v>0.87004788418025703</v>
+      </c>
+      <c r="O18" s="14">
         <f t="shared" si="3"/>
-        <v>0.82572614107883824</v>
-      </c>
-      <c r="P18" s="1">
+        <v>0.80532779385212061</v>
+      </c>
+      <c r="P18" s="6">
         <f t="shared" si="4"/>
-        <v>6.5359477124182774E-3</v>
+        <v>6.0265919559052694E-3</v>
       </c>
       <c r="Q18" s="1">
         <f t="shared" si="5"/>
-        <v>-6.639004149377592E-2</v>
-      </c>
-      <c r="R18" s="7" t="s">
+        <v>-6.4720090328136415E-2</v>
+      </c>
+      <c r="R18" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B19">
@@ -2251,54 +2245,54 @@
       <c r="E19">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F19">
-        <v>0.188</v>
-      </c>
-      <c r="G19">
-        <v>0.158</v>
-      </c>
-      <c r="H19" s="10">
-        <v>0.158</v>
+      <c r="F19" s="1">
+        <v>0.18834811000000001</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.20542531</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.15799001397439399</v>
       </c>
       <c r="I19" s="1">
-        <v>0.123</v>
-      </c>
-      <c r="J19" s="3">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="K19" s="4">
-        <v>0.104</v>
-      </c>
-      <c r="L19" s="9">
+        <v>0.123055571714343</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.13571375287857501</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.10310506328277901</v>
+      </c>
+      <c r="L19" s="6">
         <f t="shared" si="0"/>
-        <v>0.79396984924623115</v>
+        <v>0.79391966821303506</v>
       </c>
       <c r="M19" s="14">
         <f t="shared" si="1"/>
-        <v>0.61809045226130654</v>
+        <v>0.61836970710725125</v>
       </c>
       <c r="N19" s="14">
         <f t="shared" si="2"/>
-        <v>0.72340425531914898</v>
-      </c>
-      <c r="O19" s="16">
+        <v>0.72054746330385266</v>
+      </c>
+      <c r="O19" s="14">
         <f t="shared" si="3"/>
-        <v>0.55319148936170215</v>
-      </c>
-      <c r="P19" s="1">
+        <v>0.5474175625270622</v>
+      </c>
+      <c r="P19" s="6">
         <f t="shared" si="4"/>
-        <v>-0.17587939698492461</v>
+        <v>-0.1755499611057838</v>
       </c>
       <c r="Q19" s="1">
         <f t="shared" si="5"/>
-        <v>-0.17021276595744683</v>
-      </c>
-      <c r="R19" s="7" t="s">
+        <v>-0.17312990077679047</v>
+      </c>
+      <c r="R19" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B20">
@@ -2313,54 +2307,54 @@
       <c r="E20">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F20">
-        <v>0.183</v>
-      </c>
-      <c r="G20">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="H20" s="10">
-        <v>0.14199999999999999</v>
+      <c r="F20" s="1">
+        <v>0.18360599</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.17419228</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0.14162725034698501</v>
       </c>
       <c r="I20" s="1">
-        <v>0.107</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="K20" s="4">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="L20" s="9">
+        <v>0.106627718869217</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.136782468562274</v>
+      </c>
+      <c r="K20" s="1">
+        <v>9.25116893681691E-2</v>
+      </c>
+      <c r="L20" s="6">
         <f t="shared" si="0"/>
-        <v>0.69607843137254899</v>
+        <v>0.69425122719110299</v>
       </c>
       <c r="M20" s="14">
         <f t="shared" si="1"/>
-        <v>0.52450980392156865</v>
+        <v>0.52268489641773042</v>
       </c>
       <c r="N20" s="14">
         <f t="shared" si="2"/>
-        <v>0.74863387978142082</v>
-      </c>
-      <c r="O20" s="16">
+        <v>0.74497824696391435</v>
+      </c>
+      <c r="O20" s="14">
         <f t="shared" si="3"/>
-        <v>0.50273224043715847</v>
-      </c>
-      <c r="P20" s="1">
+        <v>0.5038598651828794</v>
+      </c>
+      <c r="P20" s="6">
         <f t="shared" si="4"/>
-        <v>-0.17156862745098034</v>
+        <v>-0.17156633077337258</v>
       </c>
       <c r="Q20" s="1">
         <f t="shared" si="5"/>
-        <v>-0.24590163934426235</v>
-      </c>
-      <c r="R20" s="7" t="s">
+        <v>-0.24111838178103495</v>
+      </c>
+      <c r="R20" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B21">
@@ -2375,54 +2369,54 @@
       <c r="E21">
         <v>1.49</v>
       </c>
-      <c r="F21">
-        <v>2.66</v>
-      </c>
-      <c r="G21">
-        <v>-2.1999999999999999E-2</v>
-      </c>
-      <c r="H21" s="17">
-        <v>1.08</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0.59199999999999997</v>
-      </c>
-      <c r="J21" s="20">
-        <v>1.69</v>
-      </c>
-      <c r="K21" s="4">
-        <v>-0.38400000000000001</v>
-      </c>
-      <c r="L21" s="9">
+      <c r="F21" s="1">
+        <v>2.6753994300000001</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1.81428561</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1.0764764792036099</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.59234382808919095</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1.53488578591224</v>
+      </c>
+      <c r="K21" s="1">
+        <v>-0.275293270406677</v>
+      </c>
+      <c r="L21" s="6">
         <f t="shared" si="0"/>
-        <v>0.72483221476510074</v>
+        <v>0.72246743570712069</v>
       </c>
       <c r="M21" s="14">
         <f t="shared" si="1"/>
-        <v>0.3973154362416107</v>
+        <v>0.39754619334845032</v>
       </c>
       <c r="N21" s="14">
         <f t="shared" si="2"/>
-        <v>0.63533834586466165</v>
-      </c>
-      <c r="O21" s="16">
+        <v>0.57370341366643707</v>
+      </c>
+      <c r="O21" s="14">
         <f t="shared" si="3"/>
-        <v>-0.14436090225563911</v>
-      </c>
-      <c r="P21" s="1">
+        <v>-0.10289800742264379</v>
+      </c>
+      <c r="P21" s="6">
         <f>M21-L21</f>
-        <v>-0.32751677852349004</v>
-      </c>
-      <c r="Q21" s="18">
-        <f t="shared" si="5"/>
-        <v>-0.77969924812030078</v>
-      </c>
-      <c r="R21" s="7" t="s">
+        <v>-0.32492124235867037</v>
+      </c>
+      <c r="Q21" s="3">
+        <f>O21-N21</f>
+        <v>-0.67660142108908083</v>
+      </c>
+      <c r="R21" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B22">
@@ -2437,54 +2431,54 @@
       <c r="E22">
         <v>3.42</v>
       </c>
-      <c r="F22" s="19">
-        <v>1.4</v>
-      </c>
-      <c r="G22">
-        <v>1.19</v>
-      </c>
-      <c r="H22" s="11">
-        <v>1.85</v>
+      <c r="F22" s="1">
+        <v>1.47421113</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1.5641805799999999</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1.85236602696273</v>
       </c>
       <c r="I22" s="1">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0.80300000000000005</v>
-      </c>
-      <c r="K22" s="4">
-        <v>1.9E-2</v>
-      </c>
-      <c r="L22" s="9">
+        <v>0.97845228226719205</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.72324989019201602</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.12017438548120001</v>
+      </c>
+      <c r="L22" s="6">
         <f t="shared" si="0"/>
-        <v>0.54093567251461994</v>
+        <v>0.54162749326395621</v>
       </c>
       <c r="M22" s="14">
         <f t="shared" si="1"/>
-        <v>0.28596491228070176</v>
+        <v>0.28609715855765849</v>
       </c>
       <c r="N22" s="14">
         <f t="shared" si="2"/>
-        <v>0.57357142857142862</v>
-      </c>
-      <c r="O22" s="16">
+        <v>0.4906012954820223</v>
+      </c>
+      <c r="O22" s="14">
         <f t="shared" si="3"/>
-        <v>1.3571428571428571E-2</v>
-      </c>
-      <c r="P22" s="1">
+        <v>8.1517757555663012E-2</v>
+      </c>
+      <c r="P22" s="6">
         <f t="shared" si="4"/>
-        <v>-0.25497076023391818</v>
+        <v>-0.25553033470629771</v>
       </c>
       <c r="Q22" s="1">
         <f t="shared" si="5"/>
-        <v>-0.56000000000000005</v>
-      </c>
-      <c r="R22" s="7" t="s">
+        <v>-0.40908353792635932</v>
+      </c>
+      <c r="R22" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B23">
@@ -2499,54 +2493,54 @@
       <c r="E23">
         <v>0.33200000000000002</v>
       </c>
-      <c r="F23">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="G23">
-        <v>0.39300000000000002</v>
-      </c>
-      <c r="H23" s="10">
-        <v>0.188</v>
+      <c r="F23" s="1">
+        <v>0.38419800999999998</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.39696474999999998</v>
+      </c>
+      <c r="H23" s="6">
+        <v>0.18836463447604301</v>
       </c>
       <c r="I23" s="1">
-        <v>0.252</v>
+        <v>0.25241819238494601</v>
       </c>
       <c r="J23" s="1">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="K23">
-        <v>0.248</v>
-      </c>
-      <c r="L23" s="9">
+        <v>0.16610628680722</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.24560271036432099</v>
+      </c>
+      <c r="L23" s="6">
         <f t="shared" si="0"/>
-        <v>0.56626506024096379</v>
+        <v>0.56736335685555117</v>
       </c>
       <c r="M23" s="14">
         <f t="shared" si="1"/>
-        <v>0.75903614457831325</v>
+        <v>0.76029576019562051</v>
       </c>
       <c r="N23" s="14">
         <f t="shared" si="2"/>
-        <v>0.43229166666666669</v>
-      </c>
-      <c r="O23" s="16">
+        <v>0.43234551581154734</v>
+      </c>
+      <c r="O23" s="14">
         <f t="shared" si="3"/>
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="P23" s="1">
+        <v>0.63926075609897359</v>
+      </c>
+      <c r="P23" s="6">
         <f t="shared" si="4"/>
-        <v>0.19277108433734946</v>
+        <v>0.19293240334006934</v>
       </c>
       <c r="Q23" s="1">
         <f t="shared" si="5"/>
-        <v>0.21354166666666669</v>
-      </c>
-      <c r="R23" s="7" t="s">
+        <v>0.20691524028742625</v>
+      </c>
+      <c r="R23" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B24">
@@ -2561,54 +2555,54 @@
       <c r="E24">
         <v>0.39700000000000002</v>
       </c>
-      <c r="F24">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="G24">
-        <v>0.376</v>
-      </c>
-      <c r="H24" s="10">
-        <v>0.249</v>
+      <c r="F24" s="1">
+        <v>0.66367865000000004</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.71000251000000003</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0.249323306258773</v>
       </c>
       <c r="I24" s="1">
-        <v>0.24</v>
+        <v>0.239715134888036</v>
       </c>
       <c r="J24" s="1">
-        <v>0.215</v>
-      </c>
-      <c r="K24">
-        <v>0.224</v>
-      </c>
-      <c r="L24" s="9">
+        <v>0.22804623532638299</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.23414782298617301</v>
+      </c>
+      <c r="L24" s="6">
         <f t="shared" si="0"/>
-        <v>0.62720403022670024</v>
+        <v>0.62801840367449113</v>
       </c>
       <c r="M24" s="14">
         <f t="shared" si="1"/>
-        <v>0.60453400503778332</v>
+        <v>0.6038164606751536</v>
       </c>
       <c r="N24" s="14">
         <f t="shared" si="2"/>
-        <v>0.625</v>
-      </c>
-      <c r="O24" s="16">
+        <v>0.34360941899574887</v>
+      </c>
+      <c r="O24" s="14">
         <f t="shared" si="3"/>
-        <v>0.65116279069767447</v>
-      </c>
-      <c r="P24" s="1">
+        <v>0.35280300637390249</v>
+      </c>
+      <c r="P24" s="6">
         <f t="shared" si="4"/>
-        <v>-2.267002518891692E-2</v>
+        <v>-2.4201942999337533E-2</v>
       </c>
       <c r="Q24" s="1">
         <f t="shared" si="5"/>
-        <v>2.6162790697674465E-2</v>
-      </c>
-      <c r="R24" s="7" t="s">
+        <v>9.1935873781536226E-3</v>
+      </c>
+      <c r="R24" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B25">
@@ -2623,54 +2617,54 @@
       <c r="E25">
         <v>0.46400000000000002</v>
       </c>
-      <c r="F25">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="G25">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="H25" s="10">
-        <v>0.25800000000000001</v>
+      <c r="F25" s="1">
+        <v>0.73646043999999999</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.15930865999999999</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0.257707305823206</v>
       </c>
       <c r="I25" s="1">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5339396403023403E-2</v>
       </c>
       <c r="J25" s="1">
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="K25">
-        <v>-4.9000000000000002E-2</v>
-      </c>
-      <c r="L25" s="9">
+        <v>0.31192149614585502</v>
+      </c>
+      <c r="K25" s="1">
+        <v>-1.41656022819298E-2</v>
+      </c>
+      <c r="L25" s="6">
         <f t="shared" si="0"/>
-        <v>0.55603448275862066</v>
+        <v>0.55540367634311638</v>
       </c>
       <c r="M25" s="14">
         <f t="shared" si="1"/>
-        <v>9.6982758620689641E-2</v>
+        <v>9.7714216385826294E-2</v>
       </c>
       <c r="N25" s="14">
         <f t="shared" si="2"/>
-        <v>0.63656387665198233</v>
-      </c>
-      <c r="O25" s="16">
+        <v>0.42354141404507079</v>
+      </c>
+      <c r="O25" s="14">
         <f t="shared" si="3"/>
-        <v>-0.10792951541850221</v>
-      </c>
-      <c r="P25" s="1">
+        <v>-1.923470903872284E-2</v>
+      </c>
+      <c r="P25" s="6">
         <f t="shared" si="4"/>
-        <v>-0.45905172413793105</v>
+        <v>-0.4576894599572901</v>
       </c>
       <c r="Q25" s="1">
         <f t="shared" si="5"/>
-        <v>-0.74449339207048459</v>
-      </c>
-      <c r="R25" s="7" t="s">
+        <v>-0.4427761230837936</v>
+      </c>
+      <c r="R25" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B26">
@@ -2685,49 +2679,49 @@
       <c r="E26">
         <v>0.13900000000000001</v>
       </c>
-      <c r="F26" s="21">
-        <v>0.55100000000000005</v>
-      </c>
-      <c r="G26">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="H26" s="10">
-        <v>7.3999999999999996E-2</v>
+      <c r="F26" s="1">
+        <v>0.55135862000000002</v>
+      </c>
+      <c r="G26" s="1">
+        <v>7.4029010000000006E-2</v>
+      </c>
+      <c r="H26" s="6">
+        <v>7.3876774379645099E-2</v>
       </c>
       <c r="I26" s="1">
-        <v>-0.192</v>
+        <v>-0.192488679515598</v>
       </c>
       <c r="J26" s="1">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="K26">
-        <v>-1.2E-2</v>
-      </c>
-      <c r="L26" s="9">
+        <v>7.1035866798894606E-2</v>
+      </c>
+      <c r="K26" s="1">
+        <v>-1.36594333424643E-2</v>
+      </c>
+      <c r="L26" s="6">
         <f t="shared" si="0"/>
-        <v>0.53237410071942437</v>
+        <v>0.53148758546507258</v>
       </c>
       <c r="M26" s="14">
         <f t="shared" si="1"/>
-        <v>-1.3812949640287768</v>
+        <v>-1.3848106439971077</v>
       </c>
       <c r="N26" s="14">
         <f t="shared" si="2"/>
-        <v>0.12885662431941922</v>
-      </c>
-      <c r="O26" s="16">
+        <v>0.12883786381882376</v>
+      </c>
+      <c r="O26" s="14">
         <f t="shared" si="3"/>
-        <v>-2.1778584392014518E-2</v>
-      </c>
-      <c r="P26" s="3">
+        <v>-2.477413582917104E-2</v>
+      </c>
+      <c r="P26" s="12">
         <f>M26-L26</f>
-        <v>-1.9136690647482011</v>
+        <v>-1.9162982294621802</v>
       </c>
       <c r="Q26" s="1">
         <f>O26-N26</f>
-        <v>-0.15063520871143374</v>
-      </c>
-      <c r="R26" s="7" t="s">
+        <v>-0.1536119996479948</v>
+      </c>
+      <c r="R26" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2748,49 +2742,49 @@
         <v>0.29899999999999999</v>
       </c>
       <c r="F27" s="1">
-        <v>0.34</v>
-      </c>
-      <c r="G27">
-        <v>-2.9000000000000001E-2</v>
-      </c>
-      <c r="H27" s="10">
-        <v>0.16700000000000001</v>
+        <v>0.46745129000000002</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.17633524</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0.16739930154852101</v>
       </c>
       <c r="I27" s="1">
-        <v>-0.186</v>
+        <v>-0.186311854490254</v>
       </c>
       <c r="J27" s="1">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="K27">
-        <v>-7.9000000000000001E-2</v>
-      </c>
-      <c r="L27" s="9">
+        <v>0.20967061456966801</v>
+      </c>
+      <c r="K27" s="1">
+        <v>2.0106582013602201E-2</v>
+      </c>
+      <c r="L27" s="6">
         <f t="shared" si="0"/>
-        <v>0.55852842809364556</v>
+        <v>0.55986388477766225</v>
       </c>
       <c r="M27" s="14">
         <f t="shared" si="1"/>
-        <v>-0.62207357859531776</v>
+        <v>-0.62311657020151845</v>
       </c>
       <c r="N27" s="14">
         <f t="shared" si="2"/>
-        <v>0.58529411764705885</v>
-      </c>
-      <c r="O27" s="16">
+        <v>0.44854002770998452</v>
+      </c>
+      <c r="O27" s="14">
         <f t="shared" si="3"/>
-        <v>-0.23235294117647057</v>
-      </c>
-      <c r="P27" s="1">
+        <v>4.3013213234692753E-2</v>
+      </c>
+      <c r="P27" s="6">
         <f t="shared" si="4"/>
-        <v>-1.1806020066889633</v>
+        <v>-1.1829804549791807</v>
       </c>
       <c r="Q27" s="1">
         <f t="shared" si="5"/>
-        <v>-0.81764705882352939</v>
-      </c>
-      <c r="R27" s="7" t="s">
-        <v>43</v>
+        <v>-0.40552681447529176</v>
+      </c>
+      <c r="R27" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -2810,48 +2804,48 @@
         <v>0.35699999999999998</v>
       </c>
       <c r="F28" s="1">
-        <v>0.48</v>
-      </c>
-      <c r="G28">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="H28" s="10">
-        <v>0.21199999999999999</v>
+        <v>0.60743365999999999</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.43392772000000002</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0.211769839863961</v>
       </c>
       <c r="I28" s="1">
-        <v>0.11799999999999999</v>
+        <v>0.117632335905912</v>
       </c>
       <c r="J28" s="1">
-        <v>0.27200000000000002</v>
+        <v>0.28031150580671799</v>
       </c>
       <c r="K28" s="1">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="L28" s="9">
+        <v>9.2083869813190097E-2</v>
+      </c>
+      <c r="L28" s="6">
         <f t="shared" si="0"/>
-        <v>0.5938375350140056</v>
+        <v>0.59319282875059109</v>
       </c>
       <c r="M28" s="14">
         <f t="shared" si="1"/>
-        <v>0.33053221288515405</v>
+        <v>0.32950234147314289</v>
       </c>
       <c r="N28" s="14">
         <f t="shared" si="2"/>
-        <v>0.56666666666666676</v>
-      </c>
-      <c r="O28" s="16">
+        <v>0.46146850967514375</v>
+      </c>
+      <c r="O28" s="14">
         <f t="shared" si="3"/>
-        <v>0.19375000000000001</v>
-      </c>
-      <c r="P28" s="1">
+        <v>0.15159494094085946</v>
+      </c>
+      <c r="P28" s="6">
         <f t="shared" si="4"/>
-        <v>-0.26330532212885155</v>
+        <v>-0.2636904872774482</v>
       </c>
       <c r="Q28" s="1">
         <f t="shared" si="5"/>
-        <v>-0.37291666666666679</v>
-      </c>
-      <c r="R28" s="7" t="s">
+        <v>-0.30987356873428429</v>
+      </c>
+      <c r="R28" s="5" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>